<commit_message>
dogtasCom.py iki pencerinin açılma atası giderildi.
</commit_message>
<xml_diff>
--- a/Other.xlsx
+++ b/Other.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\PRG\Fiyat\Etiket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87BDA57-6DD1-4895-BF5B-3D85CC2C3B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6322967F-E5F0-4610-B489-CF76785FE03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50547384-DF91-4631-9303-94420423840A}"/>
+    <workbookView xWindow="19320" yWindow="7560" windowWidth="7155" windowHeight="11295" xr2:uid="{50547384-DF91-4631-9303-94420423840A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,33 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>BEND Berjer</t>
+    <t>sku</t>
   </si>
   <si>
-    <t>BEND Üçlü Koltuk</t>
-  </si>
-  <si>
-    <t>BEND İkili Koltuk</t>
-  </si>
-  <si>
-    <t>BRITA Berjer</t>
-  </si>
-  <si>
-    <t>BRITA İkili Koltuk</t>
-  </si>
-  <si>
-    <t>BRITA Üçlü Koltuk</t>
-  </si>
-  <si>
-    <t>LEA Üçlü Yataklı Koltuk</t>
-  </si>
-  <si>
-    <t>LEA Berjer</t>
-  </si>
-  <si>
-    <t>LEA İkili Yataklı Koltuk</t>
+    <t>urun_adı</t>
   </si>
 </sst>
 </file>
@@ -415,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5145CD1A-4C76-4021-85F2-75761AD4259B}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,75 +407,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>3120018127</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3120018125</v>
-      </c>
-      <c r="B2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3120018129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3120016585</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3120011209</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3120011050</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3120018864</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3120019487</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3120018927</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>